<commit_message>
Reference to VD SL and unique Keys (UK) updated v1.18.2
Reference to VD SL and unique Keys (UK) updated v1.18.2
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel Details" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="127">
   <si>
     <t>Hide</t>
   </si>
@@ -576,12 +576,21 @@
   <si>
     <t>RS_VesselSizeUnit</t>
   </si>
+  <si>
+    <t>The reference from SS to the SL is throgh; Country, SpeciesListName, Year and CatchFraction</t>
+  </si>
+  <si>
+    <t>UK1</t>
+  </si>
+  <si>
+    <t>Ver 18.1.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +620,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -665,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -708,6 +732,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,10 +1023,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1144,7 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -1147,7 +1179,9 @@
         <v>11</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="16" t="s">
+        <v>125</v>
+      </c>
       <c r="D5" s="9">
         <v>3</v>
       </c>
@@ -1181,7 +1215,9 @@
         <v>11</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="21" t="s">
+        <v>125</v>
+      </c>
       <c r="D6" s="9">
         <v>4</v>
       </c>
@@ -1245,8 +1281,8 @@
     <row r="8" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="8" t="s">
-        <v>11</v>
+      <c r="C8" s="22" t="s">
+        <v>125</v>
       </c>
       <c r="D8" s="9">
         <v>6</v>
@@ -1434,6 +1470,11 @@
       </c>
       <c r="L13" s="9" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1449,8 +1490,8 @@
   </sheetPr>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1645,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="11">
@@ -1805,6 +1846,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Header text 'Short description' -> 'Field name description'
v1.18.3
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
   <si>
     <t>Hide</t>
   </si>
@@ -583,14 +583,17 @@
     <t>UK1</t>
   </si>
   <si>
-    <t>Ver 18.1.2</t>
+    <t>Field Name Description</t>
+  </si>
+  <si>
+    <t>Ver 18.1.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,6 +638,14 @@
     </font>
     <font>
       <strike/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -689,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -740,6 +751,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,7 +1041,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,8 +1066,8 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
+      <c r="E1" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
@@ -1474,7 +1489,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1506,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,8 +1534,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="E1" s="25" t="s">
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added Vocabulary code type column
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel Details" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="129">
   <si>
     <t>Hide</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Ver 18.1.3</t>
+  </si>
+  <si>
+    <t>Vocabulary code type</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -755,6 +758,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,10 +1046,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,11 +1057,12 @@
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.28515625" customWidth="1"/>
-    <col min="12" max="12" width="39.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="27"/>
+    <col min="12" max="12" width="41.28515625" customWidth="1"/>
+    <col min="13" max="13" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1084,14 +1093,17 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1118,14 +1130,15 @@
         <v>15</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1148,14 +1161,15 @@
         <v>15</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="K3" s="16"/>
       <c r="L3" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
@@ -1182,14 +1196,15 @@
       <c r="J4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1218,14 +1233,17 @@
       <c r="J5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>104</v>
+      <c r="K5" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1254,14 +1272,17 @@
       <c r="J6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1286,14 +1307,17 @@
       <c r="J7" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>115</v>
+      <c r="K7" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="M7" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="22" t="s">
@@ -1320,14 +1344,17 @@
       <c r="J8" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1352,14 +1379,15 @@
       <c r="J9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="K9" s="16"/>
       <c r="L9" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="M9" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1384,14 +1412,17 @@
       <c r="J10" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1416,14 +1447,15 @@
       <c r="J11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="16"/>
+      <c r="L11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="M11" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1448,14 +1480,15 @@
       <c r="J12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="K12" s="16"/>
       <c r="L12" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="M12" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1480,14 +1513,17 @@
       <c r="J13" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="M13" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -1503,10 +1539,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,12 +1552,13 @@
     <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="44.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="42.140625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="11" width="12.85546875" style="20" customWidth="1"/>
+    <col min="12" max="12" width="44.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1552,14 +1589,17 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1586,14 +1626,15 @@
         <v>15</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -1616,14 +1657,15 @@
         <v>15</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="K3" s="18"/>
       <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+      <c r="M3" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
@@ -1650,14 +1692,17 @@
       <c r="J4" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="23" t="s">
@@ -1685,13 +1730,16 @@
         <v>116</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" s="17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+      <c r="M5" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
@@ -1718,14 +1766,15 @@
       <c r="J6" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="17"/>
+      <c r="L6" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
@@ -1752,14 +1801,17 @@
       <c r="J7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="17" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
@@ -1786,14 +1838,17 @@
       <c r="J8" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="K8" s="13" t="s">
-        <v>33</v>
+      <c r="K8" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="11" t="s">
@@ -1820,14 +1875,17 @@
       <c r="J9" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="M9" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="11" t="s">
@@ -1854,29 +1912,32 @@
       <c r="J10" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Clean version all black text v.1.18.4
The tables have been checked and syncronised, all text is now black and the version is updated to v.1.18.4
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel Details" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="130">
   <si>
     <t>Hide</t>
   </si>
@@ -346,155 +346,12 @@
     <t>Decimal</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Encrypted vessel identifier </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max. 100 characters</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, encrypted by the national institute before it is upload. Id encrypted so that no-one can map the Id to the real vessel. This code should be used by the Encrypted Vessel Identifier field in the Vessel Selection. If the characteristics of the vessel change range group e.g. length group, then a new encrypted vessel code have to be inserted. If regional sampling schemes are use, then the vessels have to be coordinated across countries, so one vessel only appears as one record/vessel in this Vessel Details table.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ISO 3166 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>alfa-2 codes, but also e.g. GB-SCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. The country that did the sampling</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ISO 3166 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>alfa-2 codes, but also e.g. GB-SCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">he flag country of the vessel. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>String</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(100)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ISO 3166 alfa-2 codes, but also e.g. GB-SCT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Country of the species list</t>
-    </r>
-  </si>
-  <si>
     <t>ISO_3166</t>
   </si>
   <si>
     <t>Harbour_LOCODE</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">LOCODE of home </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>harbour/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>port</t>
-    </r>
-  </si>
-  <si>
     <t>EDMO</t>
   </si>
   <si>
@@ -507,70 +364,6 @@
     <t>SpecWoRMS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>table code list</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>exact</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> name of the species list</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, which each country have uploaded to the Species list SL file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>RS_VesselLengthCategory</t>
   </si>
   <si>
@@ -586,17 +379,44 @@
     <t>Field Name Description</t>
   </si>
   <si>
-    <t>Ver 18.1.3</t>
-  </si>
-  <si>
     <t>Vocabulary code type</t>
+  </si>
+  <si>
+    <t>code list</t>
+  </si>
+  <si>
+    <t>Ver 18.1.4</t>
+  </si>
+  <si>
+    <t>String(100)</t>
+  </si>
+  <si>
+    <t>Encrypted vessel identifier max. 100 characters, encrypted by the national institute before it is upload. Id encrypted so that no-one can map the Id to the real vessel. This code should be used by the Encrypted Vessel Identifier field in the Vessel Selection. If the characteristics of the vessel change range group e.g. length group, then a new encrypted vessel code have to be inserted. If regional sampling schemes are use, then the vessels have to be coordinated across countries, so one vessel only appears as one record/vessel in this Vessel Details table.</t>
+  </si>
+  <si>
+    <t>ISO 3166 alfa-2 codes, but also e.g. GB-SCT. The country that did the sampling</t>
+  </si>
+  <si>
+    <t>LOCODE of home harbour/port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO 3166 alfa-2 codes, but also e.g. GB-SCT. The flag country of the vessel. </t>
+  </si>
+  <si>
+    <t>ISO 3166 alfa-2 codes, but also e.g. GB-SCT. Country of the species list</t>
+  </si>
+  <si>
+    <t>SL table code list</t>
+  </si>
+  <si>
+    <t>The exact name of the species list, which each country have uploaded to the Species list SL file.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,37 +440,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <strike/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -703,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -721,48 +513,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,21 +817,21 @@
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="27"/>
-    <col min="12" max="12" width="41.28515625" customWidth="1"/>
-    <col min="13" max="13" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1328125" customWidth="1"/>
+    <col min="12" max="12" width="41.265625" customWidth="1"/>
+    <col min="13" max="13" width="39.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +844,8 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>126</v>
+      <c r="E1" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
@@ -1093,8 +862,8 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>128</v>
+      <c r="K1" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -1103,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1130,7 +899,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="26"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
         <v>99</v>
       </c>
@@ -1138,81 +907,81 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="9" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="9">
+        <v>117</v>
+      </c>
+      <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="M4" s="9" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="7">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1233,7 +1002,7 @@
       <c r="J5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="7" t="s">
@@ -1243,15 +1012,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1269,263 +1038,263 @@
       <c r="I6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>109</v>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="J7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="C8" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="7">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="M8" s="9" t="s">
+      <c r="J8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>7</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="9" t="s">
+      <c r="K9" s="7"/>
+      <c r="L9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="L10" s="9" t="s">
+      <c r="J10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>9</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="9" t="s">
+      <c r="K11" s="7"/>
+      <c r="L11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>10</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="9" t="s">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>11</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="L13" s="9" t="s">
+      <c r="J13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1541,24 +1310,23 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.1328125" style="2"/>
+    <col min="5" max="5" width="17.86328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="12.85546875" style="20" customWidth="1"/>
-    <col min="12" max="12" width="44.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="42.140625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="10" width="9.1328125" style="2"/>
+    <col min="11" max="11" width="14.86328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="42.1328125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1571,8 +1339,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>126</v>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1589,8 +1357,8 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>128</v>
+      <c r="K1" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -1599,7 +1367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1394,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="28"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>99</v>
       </c>
@@ -1634,315 +1402,367 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12">
         <v>1</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="12" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+    <row r="4" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="12">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12">
+        <v>5</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="12">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12">
+        <v>7</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K9" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="L9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="12">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="11">
-        <v>3</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="18" t="s">
+      <c r="L10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="11">
-        <v>4</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="11">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="11">
-        <v>6</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="11">
-        <v>7</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11">
-        <v>8</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
New versionv 1.19  no changes.
v 1.19  no changes. The striked out UK1 for VDflagCountry is removed.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC062AD-D667-4FF0-AF69-8669A3E7C015}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessel Details" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="130">
   <si>
     <t>Hide</t>
   </si>
@@ -385,9 +386,6 @@
     <t>code list</t>
   </si>
   <si>
-    <t>Ver 18.1.4</t>
-  </si>
-  <si>
     <t>String(100)</t>
   </si>
   <si>
@@ -410,12 +408,15 @@
   </si>
   <si>
     <t>The exact name of the species list, which each country have uploaded to the Species list SL file.</t>
+  </si>
+  <si>
+    <t>Ver 19.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -811,14 +812,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -957,7 +958,7 @@
         <v>74</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>15</v>
@@ -967,7 +968,7 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>70</v>
@@ -1045,7 +1046,7 @@
         <v>108</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>91</v>
@@ -1080,18 +1081,16 @@
         <v>109</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="10" t="s">
-        <v>117</v>
-      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="7">
         <v>6</v>
       </c>
@@ -1117,7 +1116,7 @@
         <v>108</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>49</v>
@@ -1294,7 +1293,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -1464,7 +1463,7 @@
         <v>108</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>87</v>
@@ -1530,11 +1529,11 @@
         <v>15</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
V1.19.1 Max values for Vessel power 9000 and Vessel tonnage 10000 updated
Vessel power max changed from 8500 kW to 9000 kW
Vessel tonnage max changed from 2500 to 10000 tonnes.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC062AD-D667-4FF0-AF69-8669A3E7C015}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D666431-D72F-49CD-830C-14B8D8FD54E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,18 +212,12 @@
     <t>VDpwr</t>
   </si>
   <si>
-    <t>4-8500</t>
-  </si>
-  <si>
     <t>power in kW, and not in a category because it is needed to calculating the kWdays.</t>
   </si>
   <si>
     <t>Engine power (kW)</t>
   </si>
   <si>
-    <t>1-2500</t>
-  </si>
-  <si>
     <t>Vessel size in tonnes</t>
   </si>
   <si>
@@ -410,7 +404,13 @@
     <t>The exact name of the species list, which each country have uploaded to the Species list SL file.</t>
   </si>
   <si>
-    <t>Ver 19.1</t>
+    <t>4-9000</t>
+  </si>
+  <si>
+    <t>1-10000</t>
+  </si>
+  <si>
+    <t>Ver 1.19.1</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +465,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,9 +526,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -533,6 +536,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,9 +824,7 @@
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -846,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
@@ -864,7 +868,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -882,7 +886,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>40</v>
@@ -902,7 +906,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>16</v>
@@ -943,35 +947,35 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
@@ -980,7 +984,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -989,13 +993,13 @@
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>15</v>
@@ -1007,10 +1011,10 @@
         <v>25</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1019,19 +1023,19 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>20</v>
@@ -1043,13 +1047,13 @@
         <v>28</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24" x14ac:dyDescent="0.45">
@@ -1078,13 +1082,13 @@
         <v>28</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.45">
@@ -1113,10 +1117,10 @@
         <v>28</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>49</v>
@@ -1139,7 +1143,7 @@
         <v>54</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>48</v>
@@ -1181,7 +1185,7 @@
         <v>28</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>60</v>
@@ -1201,7 +1205,7 @@
         <v>61</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>62</v>
@@ -1212,15 +1216,15 @@
       <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>63</v>
+      <c r="J11" s="17" t="s">
+        <v>127</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -1231,13 +1235,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>42</v>
@@ -1245,15 +1249,15 @@
       <c r="I12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>66</v>
+      <c r="J12" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
@@ -1264,13 +1268,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>20</v>
@@ -1282,13 +1286,13 @@
         <v>28</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
@@ -1339,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1357,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -1375,10 +1379,10 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1395,361 +1399,361 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="F5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K4" s="13" t="s">
+      <c r="J5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="12">
-        <v>3</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="M6" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="11">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="J8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11">
+        <v>7</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="L9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="11">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="12">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="12">
-        <v>5</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="12">
-        <v>6</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="12">
-        <v>7</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A13" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
Updated data model version
Updated data model version.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model VD SL.xlsx
+++ b/Documents/RDBES Data Model VD SL.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D666431-D72F-49CD-830C-14B8D8FD54E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018A22AA-0377-4D0D-8B45-7E1AB2822FF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
     <t>1-10000</t>
   </si>
   <si>
-    <t>Ver 1.19.1</t>
+    <t>Ver 1.19.2</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,12 +465,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +530,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,7 +818,9 @@
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1159,7 +1155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>

</xml_diff>